<commit_message>
feat: push all project changes
</commit_message>
<xml_diff>
--- a/data/generated_report.xlsx
+++ b/data/generated_report.xlsx
@@ -1728,7 +1728,7 @@
     <row r="6">
       <c r="A6" s="241" t="inlineStr">
         <is>
-          <t>ООО "АЛРОСА Информационные технологии"</t>
+          <t>ООО «АЛРОСА информационные технологии»</t>
         </is>
       </c>
       <c r="B6" s="77" t="n"/>
@@ -2175,7 +2175,11 @@
           <t>Подотчетное лицо</t>
         </is>
       </c>
-      <c r="K22" s="165" t="n"/>
+      <c r="K22" s="165" t="inlineStr">
+        <is>
+          <t>Мугинов Азат Рустамович</t>
+        </is>
+      </c>
       <c r="L22" s="77" t="n"/>
       <c r="M22" s="77" t="n"/>
       <c r="N22" s="77" t="n"/>
@@ -2202,7 +2206,11 @@
           <t>Табельный номер</t>
         </is>
       </c>
-      <c r="AR22" s="251" t="n"/>
+      <c r="AR22" s="251" t="inlineStr">
+        <is>
+          <t>D8200684</t>
+        </is>
+      </c>
       <c r="AS22" s="93" t="n"/>
       <c r="AT22" s="93" t="n"/>
       <c r="AU22" s="93" t="n"/>
@@ -4179,13 +4187,21 @@
       <c r="A67" s="267" t="n"/>
       <c r="B67" s="93" t="n"/>
       <c r="C67" s="94" t="n"/>
-      <c r="D67" s="268" t="n"/>
+      <c r="D67" s="268" t="inlineStr">
+        <is>
+          <t>25.05.2025</t>
+        </is>
+      </c>
       <c r="E67" s="93" t="n"/>
       <c r="F67" s="93" t="n"/>
       <c r="G67" s="93" t="n"/>
       <c r="H67" s="93" t="n"/>
       <c r="I67" s="94" t="n"/>
-      <c r="J67" s="65" t="n"/>
+      <c r="J67" s="65" t="inlineStr">
+        <is>
+          <t>25.05.2025</t>
+        </is>
+      </c>
       <c r="K67" s="93" t="n"/>
       <c r="L67" s="93" t="n"/>
       <c r="M67" s="93" t="n"/>
@@ -4194,7 +4210,11 @@
       <c r="P67" s="93" t="n"/>
       <c r="Q67" s="93" t="n"/>
       <c r="R67" s="93" t="n"/>
-      <c r="S67" s="269" t="n"/>
+      <c r="S67" s="269" t="inlineStr">
+        <is>
+          <t>Приказ</t>
+        </is>
+      </c>
       <c r="T67" s="93" t="n"/>
       <c r="U67" s="93" t="n"/>
       <c r="V67" s="93" t="n"/>
@@ -4303,7 +4323,11 @@
       <c r="G69" s="93" t="n"/>
       <c r="H69" s="93" t="n"/>
       <c r="I69" s="94" t="n"/>
-      <c r="J69" s="65" t="n"/>
+      <c r="J69" s="65" t="inlineStr">
+        <is>
+          <t>Суточные</t>
+        </is>
+      </c>
       <c r="K69" s="93" t="n"/>
       <c r="L69" s="93" t="n"/>
       <c r="M69" s="93" t="n"/>
@@ -4312,7 +4336,11 @@
       <c r="P69" s="93" t="n"/>
       <c r="Q69" s="93" t="n"/>
       <c r="R69" s="93" t="n"/>
-      <c r="S69" s="272" t="n"/>
+      <c r="S69" s="272" t="inlineStr">
+        <is>
+          <t>700 * 5</t>
+        </is>
+      </c>
       <c r="T69" s="93" t="n"/>
       <c r="U69" s="93" t="n"/>
       <c r="V69" s="93" t="n"/>
@@ -4320,7 +4348,9 @@
       <c r="X69" s="93" t="n"/>
       <c r="Y69" s="93" t="n"/>
       <c r="Z69" s="94" t="n"/>
-      <c r="AA69" s="258" t="n"/>
+      <c r="AA69" s="258" t="n">
+        <v>3500</v>
+      </c>
       <c r="AB69" s="93" t="n"/>
       <c r="AC69" s="93" t="n"/>
       <c r="AD69" s="93" t="n"/>

</xml_diff>

<commit_message>
feat: improve Excel report generation with numbering, ticket info, and user data
- Add automatic row numbering in column A for orders, tickets, and daily allowances
- Fix ticket date insertion in correct cell D68
- Insert order number in J67 instead of order date
- Add 'Билет' label in S68 for ticket rows
- Add sum formula in AA79 for total expenses (AA67:AA78)
- Add user full name (surname, name, patronymic) in AK81
- Improve data structure and Excel template compatibility
</commit_message>
<xml_diff>
--- a/data/generated_report.xlsx
+++ b/data/generated_report.xlsx
@@ -4184,7 +4184,9 @@
       <c r="BE66" s="94" t="n"/>
     </row>
     <row r="67" ht="38.25" customFormat="1" customHeight="1" s="160">
-      <c r="A67" s="267" t="n"/>
+      <c r="A67" s="267" t="n">
+        <v>1</v>
+      </c>
       <c r="B67" s="93" t="n"/>
       <c r="C67" s="94" t="n"/>
       <c r="D67" s="268" t="inlineStr">
@@ -4199,7 +4201,7 @@
       <c r="I67" s="94" t="n"/>
       <c r="J67" s="65" t="inlineStr">
         <is>
-          <t>25.05.2025</t>
+          <t>D820-10-0288</t>
         </is>
       </c>
       <c r="K67" s="93" t="n"/>
@@ -4255,16 +4257,26 @@
       <c r="BE67" s="94" t="n"/>
     </row>
     <row r="68" ht="48.75" customFormat="1" customHeight="1" s="160">
-      <c r="A68" s="267" t="n"/>
+      <c r="A68" s="267" t="n">
+        <v>2</v>
+      </c>
       <c r="B68" s="93" t="n"/>
       <c r="C68" s="94" t="n"/>
-      <c r="D68" s="268" t="n"/>
+      <c r="D68" s="268" t="inlineStr">
+        <is>
+          <t>21.05.2025</t>
+        </is>
+      </c>
       <c r="E68" s="93" t="n"/>
       <c r="F68" s="93" t="n"/>
       <c r="G68" s="93" t="n"/>
       <c r="H68" s="93" t="n"/>
       <c r="I68" s="94" t="n"/>
-      <c r="J68" s="63" t="n"/>
+      <c r="J68" s="63" t="inlineStr">
+        <is>
+          <t>4212125613971</t>
+        </is>
+      </c>
       <c r="K68" s="93" t="n"/>
       <c r="L68" s="93" t="n"/>
       <c r="M68" s="93" t="n"/>
@@ -4273,7 +4285,11 @@
       <c r="P68" s="93" t="n"/>
       <c r="Q68" s="93" t="n"/>
       <c r="R68" s="93" t="n"/>
-      <c r="S68" s="272" t="n"/>
+      <c r="S68" s="272" t="inlineStr">
+        <is>
+          <t>Билет</t>
+        </is>
+      </c>
       <c r="T68" s="93" t="n"/>
       <c r="U68" s="93" t="n"/>
       <c r="V68" s="93" t="n"/>
@@ -4281,7 +4297,9 @@
       <c r="X68" s="93" t="n"/>
       <c r="Y68" s="93" t="n"/>
       <c r="Z68" s="94" t="n"/>
-      <c r="AA68" s="258" t="n"/>
+      <c r="AA68" s="258" t="n">
+        <v>34366</v>
+      </c>
       <c r="AB68" s="93" t="n"/>
       <c r="AC68" s="93" t="n"/>
       <c r="AD68" s="93" t="n"/>
@@ -4314,7 +4332,9 @@
       <c r="BE68" s="94" t="n"/>
     </row>
     <row r="69" ht="48" customFormat="1" customHeight="1" s="160">
-      <c r="A69" s="267" t="n"/>
+      <c r="A69" s="267" t="n">
+        <v>3</v>
+      </c>
       <c r="B69" s="93" t="n"/>
       <c r="C69" s="94" t="n"/>
       <c r="D69" s="268" t="n"/>
@@ -4944,7 +4964,10 @@
       <c r="X79" s="31" t="n"/>
       <c r="Y79" s="31" t="n"/>
       <c r="Z79" s="31" t="n"/>
-      <c r="AA79" s="281" t="n"/>
+      <c r="AA79" s="281">
+        <f>SUM(AA67:AA78)</f>
+        <v/>
+      </c>
       <c r="AB79" s="93" t="n"/>
       <c r="AC79" s="93" t="n"/>
       <c r="AD79" s="93" t="n"/>
@@ -5004,7 +5027,11 @@
       <c r="AC81" s="77" t="n"/>
       <c r="AD81" s="77" t="n"/>
       <c r="AE81" s="77" t="n"/>
-      <c r="AK81" s="229" t="n"/>
+      <c r="AK81" s="229" t="inlineStr">
+        <is>
+          <t>Мугинов Азат Рустамович</t>
+        </is>
+      </c>
       <c r="AL81" s="77" t="n"/>
       <c r="AM81" s="77" t="n"/>
       <c r="AN81" s="77" t="n"/>

</xml_diff>